<commit_message>
finish llm tansform  check
</commit_message>
<xml_diff>
--- a/script/result_llm_tranform/autoware_docs/autoware_behavior_velocity_no_drivable_lane/result.xlsx
+++ b/script/result_llm_tranform/autoware_docs/autoware_behavior_velocity_no_drivable_lane/result.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="72">
   <si>
     <t>index</t>
   </si>
@@ -1232,10 +1232,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1390,8 +1390,8 @@
       <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>7</v>
+      <c r="H4" s="1">
+        <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>7</v>
@@ -1402,8 +1402,8 @@
       <c r="K4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>7</v>
+      <c r="L4" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="219" spans="1:12">
@@ -1428,20 +1428,20 @@
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>7</v>
+      <c r="H5" s="1">
+        <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>7</v>
+      <c r="J5" s="1">
+        <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="1" t="s">
-        <v>7</v>
+      <c r="L5" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="152" spans="1:12">
@@ -1504,20 +1504,20 @@
       <c r="G7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>7</v>
+      <c r="H7" s="1">
+        <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>7</v>
+      <c r="J7" s="1">
+        <v>1</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>7</v>
+      <c r="L7" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="236" spans="1:12">
@@ -1580,20 +1580,20 @@
       <c r="G9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>7</v>
+      <c r="H9" s="1">
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>7</v>
+      <c r="J9" s="1">
+        <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>7</v>
+      <c r="L9" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="152" spans="1:12">
@@ -1694,20 +1694,20 @@
       <c r="G12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>7</v>
+      <c r="H12" s="1">
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>7</v>
+      <c r="J12" s="1">
+        <v>1</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>7</v>
+      <c r="L12" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="13" ht="17" spans="1:12">
@@ -1898,6 +1898,34 @@
       </c>
       <c r="L17" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="8:12">
+      <c r="H18" s="1">
+        <f>COUNTIF(H2:H17,1)</f>
+        <v>6</v>
+      </c>
+      <c r="J18" s="1">
+        <f>COUNTIF(J2:J17,1)</f>
+        <v>4</v>
+      </c>
+      <c r="L18" s="1">
+        <f>COUNTIF(L2:L17,1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="8:12">
+      <c r="H19" s="1">
+        <f>COUNTIF(H2:H17,0)</f>
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <f>COUNTIF(J2:J17,0)</f>
+        <v>3</v>
+      </c>
+      <c r="L19" s="1">
+        <f>COUNTIF(L2:L17,0)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>